<commit_message>
Example added for each section
</commit_message>
<xml_diff>
--- a/dataset/combined.xlsx
+++ b/dataset/combined.xlsx
@@ -8,19 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sajed/PycharmProjects/Study-on-ChatGPT/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953DE54B-19F8-8D49-B4B8-905115ECDD92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411477B7-0799-5E4A-AF43-CF74F01BB38B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all!$N$1:$O$41</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="373">
   <si>
     <t>id</t>
   </si>
@@ -3379,9 +3395,6 @@
   </si>
   <si>
     <t>Confidence</t>
-  </si>
-  <si>
-    <t>highly confident</t>
   </si>
   <si>
     <t>Very confident</t>
@@ -4038,7 +4051,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4061,9 +4074,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -4078,9 +4088,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -4399,10 +4406,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AC41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="M18" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4423,7 +4431,7 @@
     <col min="14" max="14" width="14.1640625" style="1" customWidth="1"/>
     <col min="15" max="15" width="12.33203125" style="1" customWidth="1"/>
     <col min="16" max="16" width="12.83203125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="14" style="1" customWidth="1"/>
+    <col min="17" max="17" width="35" style="1" customWidth="1"/>
     <col min="18" max="18" width="60.1640625" style="1" customWidth="1"/>
     <col min="19" max="19" width="14.1640625" style="1" customWidth="1"/>
     <col min="20" max="20" width="12.33203125" style="1" customWidth="1"/>
@@ -4441,19 +4449,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -4465,7 +4473,7 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -4477,7 +4485,7 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="11" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="2" t="s">
@@ -4492,7 +4500,7 @@
       <c r="Q1" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="R1" s="12" t="s">
         <v>16</v>
       </c>
       <c r="S1" s="2" t="s">
@@ -4504,7 +4512,7 @@
       <c r="U1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="V1" s="12" t="s">
         <v>20</v>
       </c>
       <c r="W1" s="2" t="s">
@@ -4516,7 +4524,7 @@
       <c r="Y1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="13" t="s">
+      <c r="Z1" s="12" t="s">
         <v>24</v>
       </c>
       <c r="AA1" s="2" t="s">
@@ -4529,7 +4537,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>320</v>
       </c>
@@ -4560,20 +4568,20 @@
       <c r="K2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="M2" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>329</v>
-      </c>
       <c r="Q2" s="6" t="s">
-        <v>325</v>
+        <v>363</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>46</v>
@@ -4603,7 +4611,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>320</v>
       </c>
@@ -4638,7 +4646,7 @@
         <v>42</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>41</v>
@@ -4650,7 +4658,7 @@
         <v>52</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>325</v>
+        <v>363</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>54</v>
@@ -4680,7 +4688,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>320</v>
       </c>
@@ -4712,7 +4720,7 @@
         <v>42</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>41</v>
@@ -4721,7 +4729,7 @@
         <v>42</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>325</v>
+        <v>363</v>
       </c>
       <c r="R4" s="1" t="s">
         <v>59</v>
@@ -4751,7 +4759,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>320</v>
       </c>
@@ -4786,19 +4794,19 @@
         <v>64</v>
       </c>
       <c r="M5" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="P5" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="N5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>333</v>
-      </c>
       <c r="Q5" s="6" t="s">
-        <v>325</v>
+        <v>363</v>
       </c>
       <c r="R5" s="1" t="s">
         <v>65</v>
@@ -4828,7 +4836,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>320</v>
       </c>
@@ -4863,7 +4871,7 @@
         <v>42</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>41</v>
@@ -4872,10 +4880,10 @@
         <v>42</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="Q6" s="6" t="s">
-        <v>325</v>
+        <v>363</v>
       </c>
       <c r="R6" s="1" t="s">
         <v>71</v>
@@ -4905,7 +4913,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>320</v>
       </c>
@@ -4937,7 +4945,7 @@
         <v>45</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N7" s="3" t="s">
         <v>44</v>
@@ -4946,7 +4954,7 @@
         <v>45</v>
       </c>
       <c r="Q7" s="6" t="s">
-        <v>325</v>
+        <v>363</v>
       </c>
       <c r="R7" s="1" t="s">
         <v>77</v>
@@ -4979,7 +4987,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>321</v>
       </c>
@@ -5014,7 +5022,7 @@
         <v>42</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>41</v>
@@ -5023,10 +5031,10 @@
         <v>42</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="Q8" s="6" t="s">
-        <v>325</v>
+        <v>363</v>
       </c>
       <c r="R8" s="1" t="s">
         <v>85</v>
@@ -5059,7 +5067,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="388" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29" ht="388" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>321</v>
       </c>
@@ -5091,7 +5099,7 @@
         <v>42</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>41</v>
@@ -5100,10 +5108,10 @@
         <v>42</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="Q9" s="6" t="s">
-        <v>325</v>
+        <v>363</v>
       </c>
       <c r="R9" s="1" t="s">
         <v>90</v>
@@ -5136,7 +5144,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:29" ht="388" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" ht="388" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>321</v>
       </c>
@@ -5168,7 +5176,7 @@
         <v>42</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>41</v>
@@ -5177,10 +5185,10 @@
         <v>42</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="Q10" s="6" t="s">
-        <v>325</v>
+        <v>363</v>
       </c>
       <c r="R10" s="1" t="s">
         <v>96</v>
@@ -5210,7 +5218,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="388" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" ht="388" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>321</v>
       </c>
@@ -5242,7 +5250,7 @@
         <v>76</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>44</v>
@@ -5251,10 +5259,10 @@
         <v>45</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="Q11" s="6" t="s">
-        <v>325</v>
+        <v>363</v>
       </c>
       <c r="R11" s="1" t="s">
         <v>101</v>
@@ -5284,7 +5292,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="388" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" ht="388" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>321</v>
       </c>
@@ -5322,19 +5330,19 @@
         <v>105</v>
       </c>
       <c r="M12" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P12" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="N12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>341</v>
-      </c>
       <c r="Q12" s="6" t="s">
-        <v>325</v>
+        <v>363</v>
       </c>
       <c r="R12" s="1" t="s">
         <v>107</v>
@@ -5373,7 +5381,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>321</v>
       </c>
@@ -5411,7 +5419,7 @@
         <v>105</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>41</v>
@@ -5420,10 +5428,10 @@
         <v>42</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="Q13" s="6" t="s">
-        <v>325</v>
+        <v>363</v>
       </c>
       <c r="R13" s="1" t="s">
         <v>112</v>
@@ -5462,7 +5470,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>322</v>
       </c>
@@ -5494,7 +5502,7 @@
         <v>45</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>44</v>
@@ -5503,10 +5511,10 @@
         <v>45</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="Q14" s="6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="R14" s="1" t="s">
         <v>124</v>
@@ -5536,7 +5544,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>322</v>
       </c>
@@ -5568,7 +5576,7 @@
         <v>45</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="N15" s="1" t="s">
         <v>44</v>
@@ -5577,10 +5585,10 @@
         <v>45</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="Q15" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="R15" s="1" t="s">
         <v>129</v>
@@ -5610,7 +5618,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>322</v>
       </c>
@@ -5642,7 +5650,7 @@
         <v>42</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>41</v>
@@ -5651,10 +5659,10 @@
         <v>42</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="Q16" s="6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="R16" s="1" t="s">
         <v>134</v>
@@ -5684,8 +5692,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
+    <row r="17" spans="1:29" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
         <v>322</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -5716,7 +5724,7 @@
         <v>139</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="N17" s="1" t="s">
         <v>47</v>
@@ -5725,10 +5733,10 @@
         <v>45</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="Q17" s="6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="R17" s="1" t="s">
         <v>142</v>
@@ -5799,7 +5807,7 @@
         <v>148</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>47</v>
@@ -5808,10 +5816,10 @@
         <v>76</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="Q18" s="6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="R18" s="1" t="s">
         <v>149</v>
@@ -5850,7 +5858,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="19" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:29" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>322</v>
       </c>
@@ -5888,19 +5896,19 @@
         <v>153</v>
       </c>
       <c r="M19" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P19" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="N19" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>350</v>
-      </c>
       <c r="Q19" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="R19" s="1" t="s">
         <v>155</v>
@@ -5939,7 +5947,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="20" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:29" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>323</v>
       </c>
@@ -5974,7 +5982,7 @@
         <v>162</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="N20" s="1" t="s">
         <v>47</v>
@@ -5983,10 +5991,10 @@
         <v>42</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="Q20" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="R20" s="1" t="s">
         <v>163</v>
@@ -6025,7 +6033,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="21" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:29" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>323</v>
       </c>
@@ -6057,13 +6065,13 @@
         <v>45</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="Q21" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="R21" s="1" t="s">
         <v>169</v>
@@ -6096,7 +6104,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:29" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>323</v>
       </c>
@@ -6128,19 +6136,19 @@
         <v>42</v>
       </c>
       <c r="M22" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P22" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="N22" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O22" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P22" s="1" t="s">
-        <v>355</v>
-      </c>
       <c r="Q22" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="R22" s="1" t="s">
         <v>175</v>
@@ -6170,7 +6178,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:29" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>323</v>
       </c>
@@ -6202,7 +6210,7 @@
         <v>45</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="N23" s="1" t="s">
         <v>41</v>
@@ -6211,10 +6219,10 @@
         <v>45</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="Q23" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="R23" s="1" t="s">
         <v>180</v>
@@ -6244,7 +6252,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:29" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>323</v>
       </c>
@@ -6279,7 +6287,7 @@
         <v>45</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="N24" s="1" t="s">
         <v>44</v>
@@ -6291,7 +6299,7 @@
         <v>185</v>
       </c>
       <c r="Q24" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="R24" s="1" t="s">
         <v>187</v>
@@ -6324,7 +6332,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="25" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:29" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>323</v>
       </c>
@@ -6359,19 +6367,19 @@
         <v>42</v>
       </c>
       <c r="M25" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P25" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="N25" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O25" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P25" s="1" t="s">
-        <v>359</v>
-      </c>
       <c r="Q25" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="R25" s="1" t="s">
         <v>194</v>
@@ -6407,7 +6415,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="26" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:29" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
         <v>2.1</v>
       </c>
@@ -6433,7 +6441,7 @@
         <v>45</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="N26" s="1" t="s">
         <v>44</v>
@@ -6442,10 +6450,10 @@
         <v>45</v>
       </c>
       <c r="P26" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="Q26" s="6" t="s">
         <v>360</v>
-      </c>
-      <c r="Q26" s="6" t="s">
-        <v>361</v>
       </c>
       <c r="R26" s="1" t="s">
         <v>201</v>
@@ -6475,7 +6483,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:29" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
         <v>3.4</v>
       </c>
@@ -6508,7 +6516,7 @@
       </c>
       <c r="L27"/>
       <c r="M27" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="N27" s="1" t="s">
         <v>44</v>
@@ -6517,7 +6525,7 @@
         <v>45</v>
       </c>
       <c r="Q27" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="R27" s="1" t="s">
         <v>209</v>
@@ -6550,7 +6558,7 @@
       </c>
       <c r="AC27"/>
     </row>
-    <row r="28" spans="1:29" ht="388" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:29" ht="388" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="7">
         <v>3.5</v>
       </c>
@@ -6589,7 +6597,7 @@
         <v>45</v>
       </c>
       <c r="Q28" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="R28" s="1" t="s">
         <v>216</v>
@@ -6622,7 +6630,7 @@
       </c>
       <c r="AC28"/>
     </row>
-    <row r="29" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:29" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
         <v>3.9</v>
       </c>
@@ -6655,7 +6663,7 @@
       </c>
       <c r="L29"/>
       <c r="M29" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="N29" s="3" t="s">
         <v>44</v>
@@ -6664,7 +6672,7 @@
         <v>45</v>
       </c>
       <c r="Q29" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="R29" s="1" t="s">
         <v>223</v>
@@ -6697,7 +6705,7 @@
       </c>
       <c r="AC29"/>
     </row>
-    <row r="30" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:29" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="7">
         <v>3.9</v>
       </c>
@@ -6730,7 +6738,7 @@
       </c>
       <c r="L30"/>
       <c r="M30" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="N30" s="1" t="s">
         <v>44</v>
@@ -6739,7 +6747,7 @@
         <v>45</v>
       </c>
       <c r="Q30" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="R30" s="1" t="s">
         <v>229</v>
@@ -6772,7 +6780,7 @@
       </c>
       <c r="AC30"/>
     </row>
-    <row r="31" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:29" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
         <v>3.9</v>
       </c>
@@ -6805,7 +6813,7 @@
       </c>
       <c r="L31"/>
       <c r="M31" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="N31" s="3" t="s">
         <v>44</v>
@@ -6814,7 +6822,7 @@
         <v>45</v>
       </c>
       <c r="Q31" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="R31" s="1" t="s">
         <v>235</v>
@@ -6847,7 +6855,7 @@
       </c>
       <c r="AC31"/>
     </row>
-    <row r="32" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:29" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
         <v>3.9</v>
       </c>
@@ -6880,7 +6888,7 @@
       </c>
       <c r="L32"/>
       <c r="M32" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="N32" s="3" t="s">
         <v>44</v>
@@ -6889,7 +6897,7 @@
         <v>45</v>
       </c>
       <c r="Q32" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="R32" s="1" t="s">
         <v>241</v>
@@ -6960,7 +6968,7 @@
         <v>246</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="N33" s="1" t="s">
         <v>47</v>
@@ -6969,10 +6977,10 @@
         <v>76</v>
       </c>
       <c r="P33" s="5" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="Q33" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="R33" s="1" t="s">
         <v>248</v>
@@ -7011,9 +7019,9 @@
         <v>246</v>
       </c>
     </row>
-    <row r="34" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="9" t="s">
-        <v>373</v>
+    <row r="34" spans="1:29" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="8" t="s">
+        <v>372</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>251</v>
@@ -7043,19 +7051,19 @@
         <v>253</v>
       </c>
       <c r="M34" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P34" s="5" t="s">
         <v>371</v>
       </c>
-      <c r="N34" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="O34" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P34" s="5" t="s">
-        <v>372</v>
-      </c>
       <c r="Q34" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="R34" s="1" t="s">
         <v>255</v>
@@ -7094,7 +7102,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="35" spans="1:29" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:29" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="7">
         <v>4.0999999999999996</v>
       </c>
@@ -7171,7 +7179,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="36" spans="1:29" ht="408" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:29" ht="408" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="7">
         <v>4.2</v>
       </c>
@@ -7239,7 +7247,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="37" spans="1:29" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:29" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="7">
         <v>4.3</v>
       </c>
@@ -7319,7 +7327,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="38" spans="1:29" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:29" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="7">
         <v>4.4000000000000004</v>
       </c>
@@ -7399,7 +7407,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="39" spans="1:29" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:29" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="7">
         <v>4.5</v>
       </c>
@@ -7479,7 +7487,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="40" spans="1:29" ht="388" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:29" ht="388" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="7">
         <v>5.0999999999999996</v>
       </c>
@@ -7562,7 +7570,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="41" spans="1:29" ht="388" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:29" ht="388" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="7">
         <v>5.0999999999999996</v>
       </c>
@@ -7634,6 +7642,18 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="N1:O41" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="EPC"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="1">
+      <filters>
+        <filter val="APC"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Confidence data added for chapter 4 & 5
</commit_message>
<xml_diff>
--- a/dataset/combined.xlsx
+++ b/dataset/combined.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sajed/PycharmProjects/Study-on-ChatGPT/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C7B1B7-81F6-D84E-952D-842861403759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE70C54-0382-334E-8B2F-E8C0DC23A596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="372">
   <si>
     <t>id</t>
   </si>
@@ -2390,19 +2390,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Setting up a continuous integration (CI) server involves the following steps:
-1. Choose a CI tool, such as Jenkins, Travis CI, or CircleCI.
-2. Set up a version control system, such as Git, to manage the source code and tests.
-3. Create a simple example project with some source code and test cases.
-4. Create a configuration file (e.g. .travis.yml for Travis CI) that specifies how the CI server should build and test the project.
-5. Commit the example project and the configuration file to the version control system.
-6. Push the code to the CI server.
-7. Verify that the example project builds and tests successfully on the CI server.
-To "break the build," you can introduce a fault into the source code or add a failing test case. For example, you could change a passing test case to fail by modifying the expected output. After this, the build will fail and the CI server will notify you of the failure.
-To restore the build, you can fix the issue in the source code or test cases, and then push the changes to the version control system. The CI server will then automatically pick up the changes and run the build and tests again. If the build is successful, the CI server will notify you that the build is back to normal.
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">To set up a continuous integration (CI) server, you will need to choose a CI tool and configure it to integrate with your version control system (VCS). Popular CI tools include Jenkins, Travis CI, and CircleCI. 
 Assuming you are using Git as your VCS, you can start by creating a new repository on a hosting service such as GitHub or GitLab. Next, you can connect your CI tool to the repository by providing it with the necessary access credentials.
 Once the CI server is set up, you can begin adding your source code and tests to the repository. A simple example of source code could be a "Hello World" program written in a programming language such as Python or JavaScript. A simple test case could be a unit test that checks that the "Hello World" program returns the expected output.
@@ -2454,19 +2441,6 @@
 6. Push your changes to GitHub to trigger a new build on Travis CI. The build will fail because the test case is expecting the wrong result.
 7. To restore the build, fix the source code error or update the test case to expect the correct result. Then push the changes to GitHub and the build will pass again.
 Note: This is a simple example and there are many other possibilities when setting up a CI server, like using different languages, different CI servers, and different version control systems, but the general process is similar.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To set up a continuous integration (CI) server, you will need to first choose a CI tool such as Jenkins, Travis CI, or CircleCI. Once you have chosen a tool, you will need to set up a version control system (VCS) such as Git or Mercurial.
-1.  Install and configure the chosen CI tool on a server. 
-2.  Connect the CI tool to the chosen VCS.
-3.  Create a new repository in the VCS for the source code and another one for the tests.
-4.  Add a simple example of source code and corresponding test cases to the repositories.
-5.  Set up the CI tool to run the tests automatically whenever a change is pushed to the repository.
-6.  To experiment with "breaking the build," you can introduce a fault into the source code by causing a syntax error or adding a failing test case. 
-7.  Once the build is broken, fix the issue by correcting the error in the source code or updating the test case.
-8.  Push the changes to the repository and the CI tool should automatically run the tests again and restore the build.
-You may also want to set up notifications so that you or your team will be notified when the build is broken, and when it is restored.
-</t>
   </si>
   <si>
     <t xml:space="preserve">To set up a continuous integration (CI) server, you can use a tool like Jenkins, Travis CI, or CircleCI. These tools integrate with popular version control systems like Git and automatically build and test your code every time a change is pushed to the repository.
@@ -2641,10 +2615,6 @@
     <t>Does T1 necessarily satisfy C2? Explain.</t>
   </si>
   <si>
-    <t xml:space="preserve">No, T1 does not necessarily satisfy C2. The fact that T1 satisfies C1 does not guarantee that it will also satisfy C2, because C1 is a more comprehensive criterion that includes C2 as a subset. T1 may include additional test cases that are not covered by C2, but still meet the requirements of C1. Therefore, T1 could still provide adequate coverage according to C1 even if it does not satisfy C2.
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">(a) No, T1 does not necessarily satisfy C2. The fact that T1 satisfies C1, which subsumes C2, only means that T1 covers all the requirements specified by C2, but it does not guarantee that T1 covers all the requirements specified by C1. Therefore, T1 may or may not satisfy C2.
 </t>
   </si>
@@ -2662,11 +2632,6 @@
   </si>
   <si>
     <t>Does T2 necessarily satisfy C1? Explain.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-No, T2 does not necessarily satisfy C1. The fact that T2 satisfies C2 does not guarantee that it will also satisfy C1, because C1 is a more comprehensive criterion that includes C2 as a subset. T2 may not include test cases that are covered by C1 but not by C2, T2  may not provide adequate coverage according to C1 even if it satisfies C2.
-</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -2692,30 +2657,6 @@
   </si>
   <si>
     <t>Just says screenshot is not available.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Step by step answer.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>Better than book solution</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
   </si>
   <si>
     <r>
@@ -3857,12 +3798,59 @@
 As for the number of tests that pass the precondition and also pass the postcondition, it would depend on the specific implementation of the theory and the methods being used. Without more information, it is not possible to determine how many tests would pass both the precondition and postcondition.
 </t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Step by step answer.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Better than book solution</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Step by step answer.
+Better than book solution  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">To extend the prior exercise so that the continuous integration server uses additional verification tools such as a code coverage or static analysis tool, you would need to integrate these tools into the continuous integration pipeline. This can typically be done by configuring the CI server to run the tools as part of the build process, or by using a plugin or extension that integrates the tools directly into the CI server.
+For example, to add code coverage, you would need to configure the CI server to run a code coverage tool such as JaCoCo or Cobertura during the build process. This would typically involve adding the necessary dependencies and configuration to the build script, and then configuring the CI server to run the build script with the code coverage tool enabled.
+To add static analysis, you would need to configure the CI server to run a static analysis tool such as SonarQube or Checkstyle during the build process. This would typically involve adding the necessary dependencies and configuration to the build script, and then configuring the CI server to run the build script with the static analysis tool enabled.
+It's also worth to note that many CI servers, like Jenkins, Gitlab-CI, Travis-CI, etc, have built-in or widely supported plugin that already provide functionality of running code coverage and static analysis.
+</t>
+  </si>
+  <si>
+    <t>Suggests specific tools for code coverage &amp; static analysis</t>
+  </si>
+  <si>
+    <t>(a) T1 may or may not satisfy C2. The fact that T1 satisfies C1, which subsumes C2, means that C1 is a more comprehensive criterion that includes all of the requirements of C2. However, it does not guarantee that T1 will also satisfy C2. T1 may include test cases that are not necessary to satisfy C2, and it may not include test cases that are necessary to satisfy C2. Therefore, additional test cases may be needed to confirm that T1 also satisfies C2.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(b) No, T2 does not necessarily satisfy C1. The fact that T2 satisfies C2, which is subsumed by C1, means that T2 meets the requirements of C2 but it does not mean that T2 meets all the requirements of C1. T2 may not include test cases that are necessary to satisfy C1, and it may include test cases that are not necessary to satisfy C1. Therefore, additional test cases may be needed to confirm that T2 also satisfies C1.
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3898,6 +3886,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -4343,8 +4338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D12" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="D40" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4408,7 +4403,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="J1" s="11" t="s">
         <v>8</v>
@@ -4473,7 +4468,7 @@
     </row>
     <row r="2" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>28</v>
@@ -4485,7 +4480,7 @@
         <v>29</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>43</v>
@@ -4494,10 +4489,10 @@
         <v>44</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>42</v>
@@ -4509,7 +4504,7 @@
         <v>44</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>43</v>
@@ -4547,7 +4542,7 @@
     </row>
     <row r="3" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>30</v>
@@ -4559,7 +4554,7 @@
         <v>49</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>40</v>
@@ -4571,7 +4566,7 @@
         <v>50</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>51</v>
@@ -4583,7 +4578,7 @@
         <v>41</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>40</v>
@@ -4621,7 +4616,7 @@
     </row>
     <row r="4" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>31</v>
@@ -4633,7 +4628,7 @@
         <v>32</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>40</v>
@@ -4642,7 +4637,7 @@
         <v>41</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>55</v>
@@ -4654,7 +4649,7 @@
         <v>41</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>40</v>
@@ -4692,7 +4687,7 @@
     </row>
     <row r="5" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>33</v>
@@ -4704,7 +4699,7 @@
         <v>34</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>40</v>
@@ -4713,10 +4708,10 @@
         <v>44</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>59</v>
@@ -4731,7 +4726,7 @@
         <v>60</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>43</v>
@@ -4769,7 +4764,7 @@
     </row>
     <row r="6" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>35</v>
@@ -4781,7 +4776,7 @@
         <v>36</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>40</v>
@@ -4790,10 +4785,10 @@
         <v>41</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>64</v>
@@ -4805,7 +4800,7 @@
         <v>41</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>40</v>
@@ -4843,7 +4838,7 @@
     </row>
     <row r="7" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>37</v>
@@ -4855,7 +4850,7 @@
         <v>38</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>43</v>
@@ -4864,7 +4859,7 @@
         <v>44</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>68</v>
@@ -4876,7 +4871,7 @@
         <v>44</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>46</v>
@@ -4917,7 +4912,7 @@
     </row>
     <row r="8" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>28</v>
@@ -4929,7 +4924,7 @@
         <v>29</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>40</v>
@@ -4938,10 +4933,10 @@
         <v>41</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>76</v>
@@ -4953,7 +4948,7 @@
         <v>41</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>40</v>
@@ -4994,7 +4989,7 @@
     </row>
     <row r="9" spans="1:29" ht="388" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>30</v>
@@ -5006,7 +5001,7 @@
         <v>49</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>40</v>
@@ -5015,10 +5010,10 @@
         <v>41</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>80</v>
@@ -5030,7 +5025,7 @@
         <v>41</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>40</v>
@@ -5071,7 +5066,7 @@
     </row>
     <row r="10" spans="1:29" ht="388" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>31</v>
@@ -5083,7 +5078,7 @@
         <v>32</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>40</v>
@@ -5092,10 +5087,10 @@
         <v>41</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>85</v>
@@ -5107,7 +5102,7 @@
         <v>41</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="O10" s="3" t="s">
         <v>40</v>
@@ -5145,7 +5140,7 @@
     </row>
     <row r="11" spans="1:29" ht="388" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>33</v>
@@ -5157,7 +5152,7 @@
         <v>34</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>43</v>
@@ -5166,10 +5161,10 @@
         <v>44</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>89</v>
@@ -5181,7 +5176,7 @@
         <v>69</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>40</v>
@@ -5219,7 +5214,7 @@
     </row>
     <row r="12" spans="1:29" ht="388" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>35</v>
@@ -5231,7 +5226,7 @@
         <v>36</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>40</v>
@@ -5240,10 +5235,10 @@
         <v>41</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>94</v>
@@ -5258,7 +5253,7 @@
         <v>93</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>40</v>
@@ -5308,7 +5303,7 @@
     </row>
     <row r="13" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>37</v>
@@ -5320,7 +5315,7 @@
         <v>38</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>40</v>
@@ -5329,10 +5324,10 @@
         <v>41</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>98</v>
@@ -5347,7 +5342,7 @@
         <v>93</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="O13" s="3" t="s">
         <v>40</v>
@@ -5397,7 +5392,7 @@
     </row>
     <row r="14" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>28</v>
@@ -5409,7 +5404,7 @@
         <v>29</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>43</v>
@@ -5418,10 +5413,10 @@
         <v>44</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>109</v>
@@ -5433,7 +5428,7 @@
         <v>44</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>43</v>
@@ -5471,7 +5466,7 @@
     </row>
     <row r="15" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>30</v>
@@ -5483,7 +5478,7 @@
         <v>49</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>43</v>
@@ -5492,10 +5487,10 @@
         <v>44</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>113</v>
@@ -5507,7 +5502,7 @@
         <v>44</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>43</v>
@@ -5545,7 +5540,7 @@
     </row>
     <row r="16" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>31</v>
@@ -5557,7 +5552,7 @@
         <v>104</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>40</v>
@@ -5566,10 +5561,10 @@
         <v>41</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>117</v>
@@ -5581,7 +5576,7 @@
         <v>41</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>40</v>
@@ -5619,7 +5614,7 @@
     </row>
     <row r="17" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>33</v>
@@ -5631,7 +5626,7 @@
         <v>121</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>46</v>
@@ -5640,10 +5635,10 @@
         <v>44</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>123</v>
@@ -5655,7 +5650,7 @@
         <v>122</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="O17" s="1" t="s">
         <v>46</v>
@@ -5702,7 +5697,7 @@
     </row>
     <row r="18" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>35</v>
@@ -5714,7 +5709,7 @@
         <v>106</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>46</v>
@@ -5723,10 +5718,10 @@
         <v>69</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>129</v>
@@ -5741,7 +5736,7 @@
         <v>130</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="O18" s="3" t="s">
         <v>40</v>
@@ -5791,7 +5786,7 @@
     </row>
     <row r="19" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>37</v>
@@ -5803,7 +5798,7 @@
         <v>107</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>43</v>
@@ -5812,10 +5807,10 @@
         <v>44</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>135</v>
@@ -5830,7 +5825,7 @@
         <v>134</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="O19" s="1" t="s">
         <v>43</v>
@@ -5880,7 +5875,7 @@
     </row>
     <row r="20" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>28</v>
@@ -5892,7 +5887,7 @@
         <v>140</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>46</v>
@@ -5901,10 +5896,10 @@
         <v>41</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>141</v>
@@ -5919,7 +5914,7 @@
         <v>142</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="O20" s="1" t="s">
         <v>43</v>
@@ -5969,7 +5964,7 @@
     </row>
     <row r="21" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>30</v>
@@ -5981,13 +5976,13 @@
         <v>103</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>147</v>
@@ -5999,7 +5994,7 @@
         <v>44</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="O21" s="3" t="s">
         <v>43</v>
@@ -6040,7 +6035,7 @@
     </row>
     <row r="22" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>31</v>
@@ -6052,7 +6047,7 @@
         <v>104</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>40</v>
@@ -6061,10 +6056,10 @@
         <v>41</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>152</v>
@@ -6076,7 +6071,7 @@
         <v>41</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="O22" s="1" t="s">
         <v>40</v>
@@ -6114,7 +6109,7 @@
     </row>
     <row r="23" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>33</v>
@@ -6126,7 +6121,7 @@
         <v>105</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>40</v>
@@ -6135,10 +6130,10 @@
         <v>44</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>156</v>
@@ -6150,7 +6145,7 @@
         <v>44</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="O23" s="3" t="s">
         <v>43</v>
@@ -6188,7 +6183,7 @@
     </row>
     <row r="24" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>35</v>
@@ -6200,7 +6195,7 @@
         <v>160</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>43</v>
@@ -6212,7 +6207,7 @@
         <v>161</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>162</v>
@@ -6224,7 +6219,7 @@
         <v>44</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="O24" s="1" t="s">
         <v>43</v>
@@ -6265,7 +6260,7 @@
     </row>
     <row r="25" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>37</v>
@@ -6277,7 +6272,7 @@
         <v>107</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>40</v>
@@ -6286,10 +6281,10 @@
         <v>41</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>167</v>
@@ -6301,7 +6296,7 @@
         <v>41</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="O25" s="1" t="s">
         <v>40</v>
@@ -6351,7 +6346,7 @@
         <v>172</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>43</v>
@@ -6360,10 +6355,10 @@
         <v>44</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>173</v>
@@ -6375,7 +6370,7 @@
         <v>44</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="O26" s="1" t="s">
         <v>43</v>
@@ -6422,7 +6417,7 @@
         <v>178</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>43</v>
@@ -6431,7 +6426,7 @@
         <v>44</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>179</v>
@@ -6444,7 +6439,7 @@
       </c>
       <c r="M27"/>
       <c r="N27" s="1" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="O27" s="1" t="s">
         <v>43</v>
@@ -6504,7 +6499,7 @@
         <v>44</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>186</v>
@@ -6517,7 +6512,7 @@
       </c>
       <c r="M28"/>
       <c r="N28" s="1" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="O28" s="3" t="s">
         <v>43</v>
@@ -6571,7 +6566,7 @@
         <v>191</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>43</v>
@@ -6580,7 +6575,7 @@
         <v>44</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>192</v>
@@ -6593,7 +6588,7 @@
       </c>
       <c r="M29"/>
       <c r="N29" s="1" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="O29" s="3" t="s">
         <v>43</v>
@@ -6647,7 +6642,7 @@
         <v>196</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>43</v>
@@ -6656,7 +6651,7 @@
         <v>44</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>197</v>
@@ -6669,7 +6664,7 @@
       </c>
       <c r="M30"/>
       <c r="N30" s="1" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="O30" s="1" t="s">
         <v>43</v>
@@ -6723,7 +6718,7 @@
         <v>201</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>43</v>
@@ -6732,7 +6727,7 @@
         <v>44</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>202</v>
@@ -6745,7 +6740,7 @@
       </c>
       <c r="M31"/>
       <c r="N31" s="1" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="O31" s="3" t="s">
         <v>43</v>
@@ -6799,7 +6794,7 @@
         <v>206</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>43</v>
@@ -6808,7 +6803,7 @@
         <v>44</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>207</v>
@@ -6821,7 +6816,7 @@
       </c>
       <c r="M32"/>
       <c r="N32" s="1" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="O32" s="3" t="s">
         <v>43</v>
@@ -6875,7 +6870,7 @@
         <v>211</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>46</v>
@@ -6884,10 +6879,10 @@
         <v>69</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>213</v>
@@ -6902,7 +6897,7 @@
         <v>212</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="O33" s="3" t="s">
         <v>46</v>
@@ -6952,13 +6947,13 @@
     </row>
     <row r="34" spans="1:29" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>217</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>43</v>
@@ -6967,10 +6962,10 @@
         <v>44</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>219</v>
@@ -6985,7 +6980,7 @@
         <v>218</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="O34" s="1" t="s">
         <v>43</v>
@@ -7052,6 +7047,9 @@
       <c r="G35" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="I35" s="6" t="s">
+        <v>323</v>
+      </c>
       <c r="J35" s="1" t="s">
         <v>226</v>
       </c>
@@ -7071,7 +7069,7 @@
         <v>44</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="R35" s="1" t="s">
         <v>228</v>
@@ -7083,10 +7081,10 @@
         <v>44</v>
       </c>
       <c r="U35" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="V35" s="1" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="W35" s="1" t="s">
         <v>43</v>
@@ -7095,7 +7093,7 @@
         <v>44</v>
       </c>
       <c r="Y35" s="1" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="Z35" s="1" t="s">
         <v>229</v>
@@ -7107,7 +7105,7 @@
         <v>44</v>
       </c>
       <c r="AC35" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="36" spans="1:29" ht="408" customHeight="1" x14ac:dyDescent="0.2">
@@ -7127,47 +7125,53 @@
         <v>44</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="J36" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="L36" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="M36" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="N36" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="K36" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L36" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N36" s="1" t="s">
+      <c r="O36" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R36" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="O36" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P36" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="R36" s="1" t="s">
+      <c r="S36" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T36" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V36" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="S36" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T36" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="V36" s="1" t="s">
+      <c r="W36" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="X36" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z36" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="W36" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="X36" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z36" s="1" t="s">
-        <v>236</v>
-      </c>
       <c r="AA36" s="3" t="s">
         <v>43</v>
       </c>
@@ -7175,7 +7179,7 @@
         <v>44</v>
       </c>
       <c r="AC36" s="1" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
     </row>
     <row r="37" spans="1:29" ht="409.6" x14ac:dyDescent="0.2">
@@ -7186,19 +7190,22 @@
         <v>230</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>237</v>
+        <v>368</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>277</v>
+        <v>369</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>286</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="K37" s="1" t="s">
         <v>46</v>
@@ -7207,10 +7214,10 @@
         <v>41</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="O37" s="3" t="s">
         <v>46</v>
@@ -7219,10 +7226,10 @@
         <v>41</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="R37" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="S37" s="3" t="s">
         <v>46</v>
@@ -7231,10 +7238,10 @@
         <v>41</v>
       </c>
       <c r="U37" s="1" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="V37" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="W37" s="1" t="s">
         <v>46</v>
@@ -7243,10 +7250,10 @@
         <v>41</v>
       </c>
       <c r="Y37" s="3" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="Z37" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="AA37" s="3" t="s">
         <v>46</v>
@@ -7255,7 +7262,7 @@
         <v>41</v>
       </c>
       <c r="AC37" s="1" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
     </row>
     <row r="38" spans="1:29" ht="409.6" x14ac:dyDescent="0.2">
@@ -7263,71 +7270,74 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="D38" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="I38" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="J38" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="K38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="N38" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="J38" s="1" t="s">
+      <c r="O38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P38" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q38" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="R38" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="K38" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L38" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="M38" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="N38" s="1" t="s">
+      <c r="S38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="T38" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="U38" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="V38" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="O38" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="P38" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q38" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="R38" s="1" t="s">
+      <c r="W38" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="X38" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y38" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="Z38" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="S38" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T38" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="U38" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="V38" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="W38" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="X38" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y38" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="Z38" s="1" t="s">
-        <v>249</v>
-      </c>
       <c r="AA38" s="3" t="s">
         <v>40</v>
       </c>
@@ -7335,7 +7345,7 @@
         <v>41</v>
       </c>
       <c r="AC38" s="3" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="39" spans="1:29" ht="409.6" x14ac:dyDescent="0.2">
@@ -7343,71 +7353,74 @@
         <v>4.5</v>
       </c>
       <c r="D39" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="J39" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="K39" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="N39" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="F39" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="J39" s="1" t="s">
+      <c r="O39" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q39" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="R39" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="K39" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L39" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="M39" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="N39" s="1" t="s">
+      <c r="S39" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="T39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="U39" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="V39" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="O39" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="P39" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q39" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="R39" s="1" t="s">
+      <c r="W39" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="X39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y39" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="Z39" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="S39" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T39" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="U39" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="V39" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="W39" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="X39" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y39" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="Z39" s="1" t="s">
-        <v>256</v>
-      </c>
       <c r="AA39" s="3" t="s">
         <v>40</v>
       </c>
@@ -7415,7 +7428,7 @@
         <v>41</v>
       </c>
       <c r="AC39" s="3" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="40" spans="1:29" ht="388" customHeight="1" x14ac:dyDescent="0.2">
@@ -7426,22 +7439,28 @@
         <v>28</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="I40" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="J40" s="1" t="s">
         <v>257</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J40" s="1" t="s">
-        <v>260</v>
       </c>
       <c r="K40" s="1" t="s">
         <v>46</v>
@@ -7450,10 +7469,10 @@
         <v>41</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="O40" s="1" t="s">
         <v>46</v>
@@ -7462,10 +7481,10 @@
         <v>41</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="R40" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="S40" s="1" t="s">
         <v>46</v>
@@ -7474,10 +7493,10 @@
         <v>41</v>
       </c>
       <c r="U40" s="1" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="V40" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="W40" s="1" t="s">
         <v>46</v>
@@ -7486,10 +7505,10 @@
         <v>41</v>
       </c>
       <c r="Y40" s="1" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="Z40" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="AA40" s="1" t="s">
         <v>46</v>
@@ -7498,7 +7517,7 @@
         <v>41</v>
       </c>
       <c r="AC40" s="1" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
     </row>
     <row r="41" spans="1:29" ht="388" customHeight="1" x14ac:dyDescent="0.2">
@@ -7509,13 +7528,13 @@
         <v>30</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>266</v>
+        <v>371</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>43</v>
@@ -7523,8 +7542,11 @@
       <c r="G41" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="I41" s="6" t="s">
+        <v>285</v>
+      </c>
       <c r="J41" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="K41" s="1" t="s">
         <v>46</v>
@@ -7533,10 +7555,10 @@
         <v>44</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="N41" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="O41" s="1" t="s">
         <v>43</v>
@@ -7545,7 +7567,7 @@
         <v>44</v>
       </c>
       <c r="R41" s="1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="S41" s="1" t="s">
         <v>43</v>
@@ -7554,7 +7576,7 @@
         <v>44</v>
       </c>
       <c r="V41" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="W41" s="1" t="s">
         <v>43</v>
@@ -7563,7 +7585,7 @@
         <v>44</v>
       </c>
       <c r="Z41" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="AA41" s="1" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Added question type & reason for incorrectness column.
</commit_message>
<xml_diff>
--- a/dataset/combined.xlsx
+++ b/dataset/combined.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sajed/PycharmProjects/Study-on-ChatGPT/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F56147-EACB-DB4A-ACDA-84E25A2893D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E492A859-EEE2-DD44-8764-32C2E9B8A949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="confidence re-run" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all!$T$1:$T$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all!$H$1:$H$32</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'confidence re-run'!$I$1:$I$41</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="335">
   <si>
     <t>id</t>
   </si>
@@ -3515,6 +3515,33 @@
 This is because the equals method of Point class is being used to compare the Point and ColorPoint object, it checks for equality of x and y fields and hence the comparison returns true.
 Even though this test case does not result in an error state, it is still problematic because it can lead to unexpected behavior and bugs in the program, as it is returning true when it should be false.
 </t>
+  </si>
+  <si>
+    <t>Coding vs. Conceptual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">both </t>
+  </si>
+  <si>
+    <t>conceptual</t>
+  </si>
+  <si>
+    <t>coding</t>
+  </si>
+  <si>
+    <t>Conceptual</t>
+  </si>
+  <si>
+    <t>ChatGPT makes the wrong assumption</t>
+  </si>
+  <si>
+    <t>ChatGPT lacks the knowledge</t>
+  </si>
+  <si>
+    <t>ChatGPT lacks the knowledge &amp; ChatGPT makes the wrong assumption</t>
+  </si>
+  <si>
+    <t>Reasons if Worng</t>
   </si>
 </sst>
 </file>
@@ -4003,10 +4030,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01564EF9-5124-C249-B954-263F7E963FB7}">
-  <dimension ref="A1:AD32"/>
+  <dimension ref="A1:AF38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD34"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4015,38 +4042,39 @@
     <col min="2" max="2" width="8.83203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="45.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="46.1640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="57.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="19.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="63.5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14.1640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.33203125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="15.1640625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="65.1640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="14.1640625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.33203125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="12.83203125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="60.1640625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="14.1640625" style="1" customWidth="1"/>
-    <col min="20" max="20" width="12.33203125" style="1" customWidth="1"/>
-    <col min="21" max="22" width="12.83203125" style="1" customWidth="1"/>
-    <col min="23" max="23" width="71.33203125" style="1" customWidth="1"/>
-    <col min="24" max="24" width="14.1640625" style="1" customWidth="1"/>
-    <col min="25" max="25" width="12.33203125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="12.83203125" style="1" customWidth="1"/>
-    <col min="27" max="27" width="78.83203125" style="1" customWidth="1"/>
-    <col min="28" max="28" width="14.1640625" style="1" customWidth="1"/>
-    <col min="29" max="29" width="12.33203125" style="1" customWidth="1"/>
-    <col min="30" max="30" width="12.83203125" style="1" customWidth="1"/>
-    <col min="31" max="31" width="8.83203125" style="1" customWidth="1"/>
-    <col min="32" max="32" width="20" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28" style="1" customWidth="1"/>
+    <col min="6" max="6" width="57.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" style="1" customWidth="1"/>
+    <col min="8" max="9" width="12.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.83203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="63.5" style="1" customWidth="1"/>
+    <col min="13" max="13" width="14.1640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="15.1640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="65.1640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="14.1640625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12.33203125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="12.83203125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="60.1640625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="14.1640625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="12.33203125" style="1" customWidth="1"/>
+    <col min="23" max="24" width="12.83203125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="71.33203125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="14.1640625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="12.33203125" style="1" customWidth="1"/>
+    <col min="28" max="28" width="12.83203125" style="1" customWidth="1"/>
+    <col min="29" max="29" width="78.83203125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="14.1640625" style="1" customWidth="1"/>
+    <col min="31" max="31" width="12.33203125" style="1" customWidth="1"/>
+    <col min="32" max="32" width="12.83203125" style="1" customWidth="1"/>
     <col min="33" max="33" width="8.83203125" style="1" customWidth="1"/>
-    <col min="34" max="16384" width="8.83203125" style="1"/>
+    <col min="34" max="34" width="20" style="1" customWidth="1"/>
+    <col min="35" max="35" width="8.83203125" style="1" customWidth="1"/>
+    <col min="36" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -4059,86 +4087,92 @@
       <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="L1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="P1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="11" t="s">
+      <c r="T1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="W1" s="11" t="s">
+      <c r="Y1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="11" t="s">
+      <c r="AC1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>200</v>
       </c>
@@ -4152,67 +4186,73 @@
         <v>29</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>44</v>
+      <c r="M2" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="N2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>44</v>
+      <c r="Q2" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="R2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="S2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="W2" s="1" t="s">
+      <c r="U2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="X2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>44</v>
+      <c r="Z2" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="AA2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AB2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE2" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:32" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>200</v>
       </c>
@@ -4226,67 +4266,73 @@
         <v>49</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>41</v>
+      <c r="M3" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="N3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>41</v>
+      <c r="Q3" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="R3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="S3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="W3" s="1" t="s">
+      <c r="U3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="X3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>41</v>
+      <c r="Z3" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="AA3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC3" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AB3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC3" s="1" t="s">
+      <c r="AD3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE3" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:32" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>200</v>
       </c>
@@ -4300,64 +4346,70 @@
         <v>32</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="K4" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>41</v>
+      <c r="M4" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="N4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P4" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="O4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="R4" s="1" t="s">
+      <c r="Q4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="T4" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="S4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="W4" s="1" t="s">
+      <c r="U4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y4" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="X4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA4" s="1" t="s">
+      <c r="Z4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC4" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AB4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC4" s="3" t="s">
+      <c r="AD4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE4" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:32" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>200</v>
       </c>
@@ -4371,67 +4423,71 @@
         <v>34</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="G5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="K5" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>44</v>
+      <c r="M5" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="N5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P5" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="O5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>44</v>
+      <c r="Q5" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="R5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="S5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="T5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="W5" s="1" t="s">
+      <c r="U5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y5" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="X5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y5" s="1" t="s">
-        <v>44</v>
+      <c r="Z5" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="AA5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC5" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AB5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC5" s="1" t="s">
+      <c r="AD5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE5" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:32" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>200</v>
       </c>
@@ -4445,67 +4501,73 @@
         <v>36</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="G6" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="K6" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>41</v>
+      <c r="M6" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="N6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P6" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="O6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>41</v>
+      <c r="Q6" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="R6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T6" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="S6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="W6" s="1" t="s">
+      <c r="U6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y6" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="X6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y6" s="1" t="s">
-        <v>41</v>
+      <c r="Z6" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="AA6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AB6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC6" s="1" t="s">
+      <c r="AD6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE6" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:32" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>201</v>
       </c>
@@ -4519,67 +4581,73 @@
         <v>29</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="K7" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>41</v>
+      <c r="M7" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="N7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P7" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="O7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>41</v>
+      <c r="Q7" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="R7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T7" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="S7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="W7" s="1" t="s">
+      <c r="U7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y7" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="X7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y7" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA7" s="1" t="s">
+      <c r="Z7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC7" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AB7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC7" s="3" t="s">
+      <c r="AD7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE7" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="388" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:32" ht="388" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>201</v>
       </c>
@@ -4593,67 +4661,73 @@
         <v>49</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="G8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="K8" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K8" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="N8" s="1" t="s">
+      <c r="M8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="P8" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="O8" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="P8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="R8" s="1" t="s">
+      <c r="Q8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="T8" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="S8" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="T8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="W8" s="1" t="s">
+      <c r="U8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y8" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="X8" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA8" s="1" t="s">
+      <c r="Z8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC8" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AB8" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC8" s="3" t="s">
+      <c r="AD8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE8" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="388" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:32" ht="388" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>201</v>
       </c>
@@ -4667,67 +4741,73 @@
         <v>32</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="G9" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="K9" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="K9" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="N9" s="1" t="s">
+      <c r="M9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="P9" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="O9" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="P9" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="R9" s="1" t="s">
+      <c r="Q9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="T9" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="S9" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="T9" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="W9" s="1" t="s">
+      <c r="U9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y9" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="X9" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y9" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA9" s="1" t="s">
+      <c r="Z9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AB9" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC9" s="3" t="s">
+      <c r="AD9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE9" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="388" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:32" ht="388" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>201</v>
       </c>
@@ -4741,67 +4821,70 @@
         <v>34</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="G10" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="K10" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>44</v>
+      <c r="M10" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="N10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P10" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="O10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>44</v>
+      <c r="Q10" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="R10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T10" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="S10" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="T10" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="W10" s="1" t="s">
+      <c r="U10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y10" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="X10" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y10" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA10" s="1" t="s">
+      <c r="Z10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC10" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AB10" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC10" s="3" t="s">
+      <c r="AD10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE10" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:30" ht="388" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:32" ht="388" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>201</v>
       </c>
@@ -4815,67 +4898,73 @@
         <v>36</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="G11" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="K11" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="L11" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="K11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="N11" s="1" t="s">
+      <c r="M11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="P11" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="O11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="P11" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="R11" s="1" t="s">
+      <c r="Q11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="T11" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="S11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="T11" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="W11" s="1" t="s">
+      <c r="U11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y11" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="X11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y11" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA11" s="1" t="s">
+      <c r="Z11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC11" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="AB11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC11" s="3" t="s">
+      <c r="AD11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE11" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:32" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>202</v>
       </c>
@@ -4889,67 +4978,70 @@
         <v>29</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="G12" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="K12" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="K12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>44</v>
+      <c r="M12" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="N12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P12" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="O12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>44</v>
+      <c r="Q12" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="R12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T12" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="S12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T12" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="W12" s="1" t="s">
+      <c r="U12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y12" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="X12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y12" s="1" t="s">
-        <v>44</v>
+      <c r="Z12" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="AA12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC12" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="AB12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC12" s="1" t="s">
+      <c r="AD12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE12" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:32" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>202</v>
       </c>
@@ -4963,67 +5055,71 @@
         <v>49</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="G13" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="K13" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="K13" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="N13" s="1" t="s">
+      <c r="M13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="P13" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="O13" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="P13" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="R13" s="1" t="s">
+      <c r="Q13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="T13" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="S13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="W13" s="1" t="s">
+      <c r="U13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y13" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="X13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y13" s="1" t="s">
-        <v>41</v>
+      <c r="Z13" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="AA13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC13" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="AB13" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC13" s="3" t="s">
+      <c r="AD13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE13" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:32" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>202</v>
       </c>
@@ -5037,67 +5133,73 @@
         <v>90</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="G14" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="K14" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="K14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="N14" s="1" t="s">
+      <c r="M14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="P14" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="O14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="P14" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="R14" s="1" t="s">
+      <c r="Q14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="R14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="T14" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="S14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="T14" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="W14" s="1" t="s">
+      <c r="U14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y14" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="X14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y14" s="1" t="s">
-        <v>41</v>
+      <c r="Z14" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="AA14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC14" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="AB14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC14" s="1" t="s">
+      <c r="AD14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE14" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:32" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>202</v>
       </c>
@@ -5111,67 +5213,70 @@
         <v>106</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="G15" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="K15" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="L15" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="K15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>41</v>
+      <c r="M15" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="N15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P15" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="O15" s="3" t="s">
+      <c r="Q15" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="P15" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="R15" s="1" t="s">
+      <c r="R15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="T15" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="S15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="W15" s="1" t="s">
+      <c r="U15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y15" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="X15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y15" s="1" t="s">
-        <v>41</v>
+      <c r="Z15" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="AA15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC15" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="AB15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC15" s="1" t="s">
+      <c r="AD15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE15" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:32" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>202</v>
       </c>
@@ -5185,67 +5290,73 @@
         <v>92</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="G16" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="I16" s="5" t="s">
+      <c r="K16" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="L16" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="K16" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="L16" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="N16" s="1" t="s">
+      <c r="M16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="P16" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="O16" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="P16" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="R16" s="1" t="s">
+      <c r="Q16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="T16" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="S16" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="T16" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="W16" s="1" t="s">
+      <c r="U16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y16" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="X16" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y16" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA16" s="1" t="s">
+      <c r="Z16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC16" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="AB16" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC16" s="3" t="s">
+      <c r="AD16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE16" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:32" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>203</v>
       </c>
@@ -5259,67 +5370,73 @@
         <v>116</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="H17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="J17" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="K17" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="L17" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="M17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="N17" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="N17" s="1" t="s">
+      <c r="P17" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="O17" s="1" t="s">
+      <c r="Q17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P17" s="1" t="s">
+      <c r="R17" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="R17" s="1" t="s">
+      <c r="T17" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="S17" s="1" t="s">
+      <c r="U17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="T17" s="1" t="s">
+      <c r="V17" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="W17" s="1" t="s">
+      <c r="Y17" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="X17" s="1" t="s">
+      <c r="Z17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="Y17" s="1" t="s">
+      <c r="AA17" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AA17" s="1" t="s">
+      <c r="AC17" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="AB17" s="1" t="s">
+      <c r="AD17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AC17" s="1" t="s">
+      <c r="AE17" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:32" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>203</v>
       </c>
@@ -5333,67 +5450,70 @@
         <v>89</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="G18" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J18" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="I18" s="5" t="s">
+      <c r="K18" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="L18" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="K18" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>44</v>
+      <c r="M18" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="N18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P18" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="O18" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P18" s="1" t="s">
-        <v>44</v>
+      <c r="Q18" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="R18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T18" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="S18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T18" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="W18" s="1" t="s">
+      <c r="U18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y18" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="X18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y18" s="1" t="s">
-        <v>41</v>
+      <c r="Z18" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="AA18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC18" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="AB18" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC18" s="1" t="s">
+      <c r="AD18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE18" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:32" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>203</v>
       </c>
@@ -5407,67 +5527,73 @@
         <v>90</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="G19" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="J19" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="I19" s="5" t="s">
+      <c r="K19" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="L19" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="K19" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="N19" s="1" t="s">
+      <c r="M19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="P19" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="O19" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="P19" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="R19" s="1" t="s">
+      <c r="Q19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="R19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="T19" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="S19" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="T19" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="W19" s="1" t="s">
+      <c r="U19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y19" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="X19" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y19" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA19" s="1" t="s">
+      <c r="Z19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC19" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="AB19" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC19" s="3" t="s">
+      <c r="AD19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE19" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:32" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>203</v>
       </c>
@@ -5481,67 +5607,70 @@
         <v>91</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="G20" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J20" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="I20" s="5" t="s">
+      <c r="K20" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="L20" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="K20" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>44</v>
+      <c r="M20" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="N20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P20" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="O20" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>44</v>
+      <c r="Q20" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="R20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T20" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="S20" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T20" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="W20" s="1" t="s">
+      <c r="U20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y20" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="X20" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y20" s="1" t="s">
-        <v>44</v>
+      <c r="Z20" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="AA20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC20" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="AB20" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC20" s="1" t="s">
+      <c r="AD20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE20" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:32" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>203</v>
       </c>
@@ -5555,106 +5684,112 @@
         <v>133</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="G21" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J21" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="I21" s="5" t="s">
+      <c r="K21" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="L21" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="K21" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>44</v>
+      <c r="M21" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="N21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P21" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="O21" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>44</v>
+      <c r="Q21" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="R21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T21" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="S21" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T21" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="W21" s="1" t="s">
+      <c r="U21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y21" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="X21" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y21" s="1" t="s">
-        <v>44</v>
+      <c r="Z21" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="AA21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC21" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="AB21" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC21" s="1" t="s">
+      <c r="AD21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE21" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:32" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>2.1</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="I22" s="5"/>
-      <c r="R22" s="1" t="s">
+      <c r="E22" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="K22" s="5"/>
+      <c r="T22" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="S22" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T22" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="V22" s="5" t="s">
+      <c r="U22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="X22" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="W22" s="1" t="s">
+      <c r="Y22" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="X22" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y22" s="1" t="s">
-        <v>44</v>
+      <c r="Z22" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="AA22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC22" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="AB22" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC22" s="1" t="s">
+      <c r="AD22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE22" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:32" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>3.4</v>
       </c>
@@ -5664,42 +5799,45 @@
       <c r="D23" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="M23"/>
-      <c r="Q23"/>
-      <c r="R23" s="1" t="s">
+      <c r="E23" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="O23"/>
+      <c r="S23"/>
+      <c r="T23" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="S23" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T23" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="V23" s="5" t="s">
+      <c r="U23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="X23" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="W23" s="1" t="s">
+      <c r="Y23" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="X23" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y23" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z23"/>
+      <c r="Z23" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="AA23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB23"/>
+      <c r="AC23" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="AB23" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC23" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD23"/>
+      <c r="AD23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF23"/>
     </row>
-    <row r="24" spans="1:30" ht="388" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:32" ht="388" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>3.5</v>
       </c>
@@ -5709,46 +5847,49 @@
       <c r="D24" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="Q24"/>
-      <c r="R24" s="1" t="s">
+      <c r="E24" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24"/>
+      <c r="T24" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="S24" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T24" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="V24" s="5" t="s">
+      <c r="U24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="X24" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="W24" s="1" t="s">
+      <c r="Y24" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="X24" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y24" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z24"/>
+      <c r="Z24" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="AA24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB24"/>
+      <c r="AC24" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="AB24" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC24" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD24"/>
+      <c r="AD24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF24"/>
     </row>
-    <row r="25" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:32" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>3.9</v>
       </c>
@@ -5762,70 +5903,73 @@
         <v>152</v>
       </c>
       <c r="E25" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="G25" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I25" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K25" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="L25" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="K25" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="M25"/>
+      <c r="M25" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="N25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O25"/>
+      <c r="P25" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="O25" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P25" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q25"/>
+      <c r="Q25" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="R25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S25"/>
+      <c r="T25" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="S25" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T25" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U25"/>
-      <c r="V25"/>
-      <c r="W25" s="1" t="s">
+      <c r="U25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="W25"/>
+      <c r="X25"/>
+      <c r="Y25" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="X25" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y25" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z25"/>
+      <c r="Z25" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="AA25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB25"/>
+      <c r="AC25" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="AB25" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC25" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD25"/>
+      <c r="AD25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF25"/>
     </row>
-    <row r="26" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:32" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>3.9</v>
       </c>
@@ -5839,70 +5983,73 @@
         <v>157</v>
       </c>
       <c r="E26" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="G26" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I26" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K26" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="L26" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="K26" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="M26"/>
+      <c r="M26" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="N26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O26"/>
+      <c r="P26" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="O26" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P26" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q26"/>
+      <c r="Q26" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="R26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S26"/>
+      <c r="T26" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="S26" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T26" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U26"/>
-      <c r="V26"/>
-      <c r="W26" s="1" t="s">
+      <c r="U26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="W26"/>
+      <c r="X26"/>
+      <c r="Y26" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="X26" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y26" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z26"/>
+      <c r="Z26" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="AA26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB26"/>
+      <c r="AC26" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="AB26" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC26" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD26"/>
+      <c r="AD26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF26"/>
     </row>
-    <row r="27" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:32" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <v>3.9</v>
       </c>
@@ -5916,70 +6063,73 @@
         <v>162</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="G27" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I27" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K27" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="L27" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="K27" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L27" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="M27"/>
+      <c r="M27" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="N27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O27"/>
+      <c r="P27" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="O27" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P27" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q27"/>
+      <c r="Q27" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="R27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S27"/>
+      <c r="T27" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="S27" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T27" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U27"/>
-      <c r="V27"/>
-      <c r="W27" s="1" t="s">
+      <c r="U27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="W27"/>
+      <c r="X27"/>
+      <c r="Y27" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="X27" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y27" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z27"/>
+      <c r="Z27" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="AA27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB27"/>
+      <c r="AC27" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="AB27" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC27" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD27"/>
+      <c r="AD27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF27"/>
     </row>
-    <row r="28" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:32" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>3.9</v>
       </c>
@@ -5993,70 +6143,73 @@
         <v>167</v>
       </c>
       <c r="E28" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="G28" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I28" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K28" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="L28" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="K28" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="M28"/>
+      <c r="M28" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="N28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O28"/>
+      <c r="P28" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="O28" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q28"/>
+      <c r="Q28" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="R28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S28"/>
+      <c r="T28" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="S28" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T28" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U28"/>
-      <c r="V28"/>
-      <c r="W28" s="1" t="s">
+      <c r="U28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="W28"/>
+      <c r="X28"/>
+      <c r="Y28" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="X28" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y28" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z28"/>
+      <c r="Z28" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="AA28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB28"/>
+      <c r="AC28" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="AB28" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC28" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD28"/>
+      <c r="AD28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF28"/>
     </row>
-    <row r="29" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:32" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
         <v>3.9</v>
       </c>
@@ -6070,70 +6223,73 @@
         <v>172</v>
       </c>
       <c r="E29" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="H29" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H29" s="13" t="s">
+      <c r="J29" s="13" t="s">
         <v>266</v>
       </c>
-      <c r="I29" s="1" t="s">
+      <c r="K29" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="L29" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="K29" s="1" t="s">
+      <c r="M29" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L29" s="1" t="s">
+      <c r="N29" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="N29" s="1" t="s">
+      <c r="P29" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="O29" s="1" t="s">
+      <c r="Q29" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P29" s="1" t="s">
+      <c r="R29" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="Q29" s="3"/>
-      <c r="R29" s="1" t="s">
+      <c r="S29" s="3"/>
+      <c r="T29" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="S29" s="1" t="s">
+      <c r="U29" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="T29" s="1" t="s">
+      <c r="V29" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="W29" s="1" t="s">
+      <c r="Y29" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="X29" s="1" t="s">
+      <c r="Z29" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="Y29" s="1" t="s">
+      <c r="AA29" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="Z29" s="3"/>
-      <c r="AA29" s="1" t="s">
+      <c r="AB29" s="3"/>
+      <c r="AC29" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="AB29" s="1" t="s">
+      <c r="AD29" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AC29" s="1" t="s">
+      <c r="AE29" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AD29" s="3"/>
+      <c r="AF29" s="3"/>
     </row>
-    <row r="30" spans="1:30" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:32" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
         <v>4.0999999999999996</v>
       </c>
@@ -6143,39 +6299,42 @@
       <c r="D30" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="I30" s="5"/>
-      <c r="R30" s="1" t="s">
+      <c r="E30" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="K30" s="5"/>
+      <c r="T30" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="S30" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T30" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="V30" s="5" t="s">
+      <c r="U30" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V30" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="X30" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="W30" s="1" t="s">
+      <c r="Y30" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="X30" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y30" s="1" t="s">
-        <v>44</v>
+      <c r="Z30" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="AA30" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC30" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="AB30" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC30" s="1" t="s">
+      <c r="AD30" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE30" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:30" ht="388" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:32" ht="388" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
         <v>5.0999999999999996</v>
       </c>
@@ -6189,67 +6348,73 @@
         <v>186</v>
       </c>
       <c r="E31" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G31" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="H31" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="J31" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="I31" s="5" t="s">
+      <c r="K31" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="J31" s="1" t="s">
+      <c r="L31" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="K31" s="1" t="s">
+      <c r="M31" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L31" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="N31" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P31" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="O31" s="1" t="s">
+      <c r="Q31" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P31" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="R31" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T31" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="S31" s="1" t="s">
+      <c r="U31" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="T31" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="W31" s="1" t="s">
+      <c r="V31" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y31" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="X31" s="1" t="s">
+      <c r="Z31" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="Y31" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="AA31" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC31" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="AB31" s="1" t="s">
+      <c r="AD31" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AC31" s="1" t="s">
+      <c r="AE31" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:30" ht="388" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:32" ht="388" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
         <v>5.0999999999999996</v>
       </c>
@@ -6263,61 +6428,94 @@
         <v>192</v>
       </c>
       <c r="E32" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="G32" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I32" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K32" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="J32" s="1" t="s">
+      <c r="L32" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="K32" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L32" s="1" t="s">
-        <v>44</v>
+      <c r="M32" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="N32" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P32" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="O32" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P32" s="1" t="s">
-        <v>44</v>
+      <c r="Q32" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="R32" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T32" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="S32" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T32" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="W32" s="1" t="s">
+      <c r="U32" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V32" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y32" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="X32" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y32" s="1" t="s">
-        <v>44</v>
+      <c r="Z32" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="AA32" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC32" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="AB32" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC32" s="1" t="s">
-        <v>44</v>
+      <c r="AD32" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE32" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E36" s="1">
+        <f>COUNTIF(E2:E32,"coding")</f>
+        <v>6</v>
+      </c>
+      <c r="I36" s="1">
+        <f>COUNTIF(I1:I31,"ChatGPT lacks the knowledge")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E37" s="1">
+        <f>COUNTIF(E2:E32,"conceptual")</f>
+        <v>9</v>
+      </c>
+      <c r="I37" s="1">
+        <f>COUNTIF(I2:I31,"ChatGPT makes the wrong assumption")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E38" s="1">
+        <f>COUNTIF(E2:E32,"both ")</f>
+        <v>16</v>
+      </c>
+      <c r="I38" s="1">
+        <f>COUNTIF(I2:I31,"ChatGPT lacks the knowledge &amp; ChatGPT makes the wrong assumption")</f>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Analysis on code vs conceptual
</commit_message>
<xml_diff>
--- a/dataset/combined.xlsx
+++ b/dataset/combined.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sajed/PycharmProjects/Study-on-ChatGPT/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E492A859-EEE2-DD44-8764-32C2E9B8A949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A158FCB5-BDDF-EE42-8D1A-C8A16C39A070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="confidence re-run" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all!$H$1:$H$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all!$I$1:$I$38</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'confidence re-run'!$I$1:$I$41</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -4032,8 +4032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01564EF9-5124-C249-B954-263F7E963FB7}">
   <dimension ref="A1:AF38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="D32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>